<commit_message>
subir el word de frances y avances en webapi
</commit_message>
<xml_diff>
--- a/Git/Git Comandos.xlsx
+++ b/Git/Git Comandos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://softwareone-my.sharepoint.com/personal/juan_morales1_softwareone_com/Documents/Documents/Clases/Git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan.morales1\Documents\Clasess\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{EDFAA0D6-803A-461F-BE33-67A53995CBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C736DCED-60E8-4235-B51D-382D0DEAC6B7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB3E3B9-955E-4B88-9CFB-A4C25960E4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Comando</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>muestra la diferencia hecha en un archivo, mas especifico que el estatus</t>
+  </si>
+  <si>
+    <t>git rm .env --cached</t>
+  </si>
+  <si>
+    <t>esto se hace cuando en el .gitignore quiero ignorar un archivo que ya subi anteriormente, reemplazo el .env con el nombre del archivo, luego hago el .add commit y push</t>
   </si>
 </sst>
 </file>
@@ -471,13 +477,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
@@ -650,7 +656,16 @@
         <v>40</v>
       </c>
     </row>
+    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>